<commit_message>
Made image import easier and replaced event images with higher quality versions, and added a favicon.
</commit_message>
<xml_diff>
--- a/project/frontend/src/assets/image_labels/image_label.xlsx
+++ b/project/frontend/src/assets/image_labels/image_label.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexung/Desktop/data-science-project/project/frontend/src/assets/image_labels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://verovis-my.sharepoint.com/personal/maurice_schmetzer_df_valantic_com/Documents/Valantic Digital Finance/Visual Studio Code/Workspace/data-science-project/project/frontend/src/assets/image_labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D51E716-567D-7349-91D4-EC4292F2C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{0D51E716-567D-7349-91D4-EC4292F2C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4436D10-1B24-460A-A652-A0291EF77C96}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{5B3E0AEF-9044-7143-BC7B-CE2F8A4714A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5B3E0AEF-9044-7143-BC7B-CE2F8A4714A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$B$51</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Event type</t>
   </si>
@@ -185,9 +188,6 @@
     <t>german_course</t>
   </si>
   <si>
-    <t>Local Tübingen festivals, city celebrations, or public cultural events.</t>
-  </si>
-  <si>
     <t>University open days, campus tours, or informational orientation events.</t>
   </si>
   <si>
@@ -296,9 +296,6 @@
     <t>Informational sessions explaining programs, opportunities, or administrative topics.</t>
   </si>
   <si>
-    <t>Research fairs showcasing scientific projects, posters, or student research.</t>
-  </si>
-  <si>
     <t>Talks or presentations by companies about careers, projects, or industry insights.</t>
   </si>
   <si>
@@ -318,13 +315,43 @@
   </si>
   <si>
     <t>Library-related events, study sessions, or academic resource introductions.</t>
+  </si>
+  <si>
+    <t>resume_workshop</t>
+  </si>
+  <si>
+    <t>Workshop about job applications, cvs, cover letters, or career preparation</t>
+  </si>
+  <si>
+    <t>science_fair</t>
+  </si>
+  <si>
+    <t>Research fairs showcasing broard research projects, posters, or student research.</t>
+  </si>
+  <si>
+    <t>Science fairs showcasing scientific specific projects &amp; discoveries</t>
+  </si>
+  <si>
+    <t>festival</t>
+  </si>
+  <si>
+    <t>Local Tuebingen festivals, city celebrations, or public cultural events.</t>
+  </si>
+  <si>
+    <t>General festival that is not related to tuebingen.</t>
+  </si>
+  <si>
+    <t>graduation</t>
+  </si>
+  <si>
+    <t>Events related to university graduation and finishing studies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -332,19 +359,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -361,10 +390,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -379,8 +408,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -696,19 +729,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54404864-E03E-E243-BAAA-7B6942057DC3}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="155.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="75.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -716,375 +749,413 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B32" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>65</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B51" xr:uid="{54404864-E03E-E243-BAAA-7B6942057DC3}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B51">
+      <sortCondition ref="A1:A51"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
handled online events and updated images for consistency
</commit_message>
<xml_diff>
--- a/project/frontend/src/assets/image_labels/image_label.xlsx
+++ b/project/frontend/src/assets/image_labels/image_label.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://verovis-my.sharepoint.com/personal/maurice_schmetzer_df_valantic_com/Documents/Valantic Digital Finance/Visual Studio Code/Workspace/data-science-project/project/frontend/src/assets/image_labels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitc-my.sharepoint.com/personal/zxoqk56_s-cloud_uni-tuebingen_de/Documents/third_semester/DSP/data-science-project/project/frontend/src/assets/image_labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{0D51E716-567D-7349-91D4-EC4292F2C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4436D10-1B24-460A-A652-A0291EF77C96}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{0D51E716-567D-7349-91D4-EC4292F2C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78908D36-D9FA-43C1-BBBB-3BC73EA9E01C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5B3E0AEF-9044-7143-BC7B-CE2F8A4714A9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5B3E0AEF-9044-7143-BC7B-CE2F8A4714A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$B$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$B$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Event type</t>
   </si>
@@ -323,21 +323,12 @@
     <t>Workshop about job applications, cvs, cover letters, or career preparation</t>
   </si>
   <si>
-    <t>science_fair</t>
-  </si>
-  <si>
     <t>Research fairs showcasing broard research projects, posters, or student research.</t>
   </si>
   <si>
-    <t>Science fairs showcasing scientific specific projects &amp; discoveries</t>
-  </si>
-  <si>
     <t>festival</t>
   </si>
   <si>
-    <t>Local Tuebingen festivals, city celebrations, or public cultural events.</t>
-  </si>
-  <si>
     <t>General festival that is not related to tuebingen.</t>
   </si>
   <si>
@@ -345,6 +336,9 @@
   </si>
   <si>
     <t>Events related to university graduation and finishing studies</t>
+  </si>
+  <si>
+    <t>Local Tuebingen festivals, city celebrations.</t>
   </si>
 </sst>
 </file>
@@ -729,19 +723,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54404864-E03E-E243-BAAA-7B6942057DC3}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="75.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,7 +743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -757,7 +751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -765,7 +759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -773,7 +767,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -781,7 +775,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -789,7 +783,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -797,7 +791,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -805,7 +799,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -813,7 +807,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -821,7 +815,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -829,7 +823,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>73</v>
       </c>
@@ -837,7 +831,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -845,7 +839,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -853,7 +847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -861,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -869,7 +863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -877,7 +871,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -885,23 +879,23 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -909,7 +903,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -917,7 +911,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -925,15 +919,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -941,7 +935,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -949,7 +943,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -957,7 +951,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -965,7 +959,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -973,7 +967,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -981,7 +975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -989,7 +983,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -997,7 +991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -1005,7 +999,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1013,7 +1007,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1021,7 +1015,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1029,7 +1023,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -1037,7 +1031,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -1045,15 +1039,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>92</v>
       </c>
@@ -1061,7 +1055,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -1069,90 +1063,82 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>66</v>
-      </c>
-      <c r="B51" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B51" xr:uid="{54404864-E03E-E243-BAAA-7B6942057DC3}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B51">
-      <sortCondition ref="A1:A51"/>
+  <autoFilter ref="A1:B50" xr:uid="{54404864-E03E-E243-BAAA-7B6942057DC3}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B50">
+      <sortCondition ref="A1:A50"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>